<commit_message>
Update README.md + Update of all files to be fully functional with a new environment set up
</commit_message>
<xml_diff>
--- a/data/Appendix 4 - Data for simulations.xlsx
+++ b/data/Appendix 4 - Data for simulations.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\MyWork\Reviews\Game theory paper - Jakob\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Game_theory_rabies\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843C01C4-6B55-4112-90B0-9704638D28D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120"/>
+    <workbookView xWindow="9585" yWindow="1830" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pop_Data" sheetId="1" r:id="rId1"/>
     <sheet name="AVG_HCE_Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="169">
   <si>
     <t>iso_a2</t>
   </si>
@@ -523,18 +535,29 @@
   </si>
   <si>
     <t>probability_pep_ub</t>
+  </si>
+  <si>
+    <t>human_population_2024</t>
+  </si>
+  <si>
+    <t>gdp_per_capita_20224</t>
+  </si>
+  <si>
+    <t>gdp_2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="165" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_ * #,##0.000_ ;_ * \-#,##0.000_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,6 +593,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -597,17 +626,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -619,23 +649,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Comma 2" xfId="2"/>
+  <cellStyles count="4">
+    <cellStyle name="Comma 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Milliers" xfId="3" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -912,14 +949,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="X1" sqref="X1:X1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.125" style="3" bestFit="1" customWidth="1"/>
@@ -938,10 +975,14 @@
     <col min="16" max="16" width="15" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="3"/>
+    <col min="19" max="21" width="9" style="3"/>
+    <col min="22" max="22" width="22.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
@@ -1005,8 +1046,17 @@
       <c r="U1" s="3" t="s">
         <v>162</v>
       </c>
+      <c r="V1" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>168</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1070,8 +1120,17 @@
       <c r="U2" s="3">
         <v>150</v>
       </c>
+      <c r="V2" s="10">
+        <v>46731365.000000015</v>
+      </c>
+      <c r="W2" s="3">
+        <v>4114.1549906144819</v>
+      </c>
+      <c r="X2" s="11">
+        <v>192260078532.97699</v>
+      </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1135,8 +1194,17 @@
       <c r="U3" s="3">
         <v>150</v>
       </c>
+      <c r="V3" s="10">
+        <v>37298625</v>
+      </c>
+      <c r="W3" s="3">
+        <v>2336.1513177117904</v>
+      </c>
+      <c r="X3" s="11">
+        <v>87135231942.587921</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1200,8 +1268,17 @@
       <c r="U4" s="3">
         <v>150</v>
       </c>
+      <c r="V4" s="10">
+        <v>13470099.999999998</v>
+      </c>
+      <c r="W4" s="3">
+        <v>1560.9027980683363</v>
+      </c>
+      <c r="X4" s="11">
+        <v>21025516780.260296</v>
+      </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1265,8 +1342,17 @@
       <c r="U5" s="3">
         <v>150</v>
       </c>
+      <c r="V5" s="10">
+        <v>2525764.9999999995</v>
+      </c>
+      <c r="W5" s="3">
+        <v>8028.8688720748514</v>
+      </c>
+      <c r="X5" s="11">
+        <v>20279035986.676132</v>
+      </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1416,17 @@
       <c r="U6" s="3">
         <v>150</v>
       </c>
+      <c r="V6" s="10">
+        <v>23351513.000000019</v>
+      </c>
+      <c r="W6" s="3">
+        <v>1003.2901163852914</v>
+      </c>
+      <c r="X6" s="11">
+        <v>23428342195.542664</v>
+      </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1395,8 +1490,17 @@
       <c r="U7" s="3">
         <v>150</v>
       </c>
+      <c r="V7" s="10">
+        <v>13378732.000000002</v>
+      </c>
+      <c r="W7" s="3">
+        <v>258.75274253438215</v>
+      </c>
+      <c r="X7" s="11">
+        <v>3461783596.6325002</v>
+      </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>19</v>
       </c>
@@ -1460,8 +1564,17 @@
       <c r="U8" s="3">
         <v>150</v>
       </c>
+      <c r="V8" s="10">
+        <v>29314689.000000004</v>
+      </c>
+      <c r="W8" s="3">
+        <v>1815.7867563857214</v>
+      </c>
+      <c r="X8" s="11">
+        <v>53229224053.766197</v>
+      </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1525,8 +1638,17 @@
       <c r="U9" s="3">
         <v>150</v>
       </c>
+      <c r="V9" s="10">
+        <v>5226574.0000000019</v>
+      </c>
+      <c r="W9" s="3">
+        <v>558.91319159676959</v>
+      </c>
+      <c r="X9" s="11">
+        <v>2921201155.4566956</v>
+      </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
@@ -1590,8 +1712,17 @@
       <c r="U10" s="3">
         <v>150</v>
       </c>
+      <c r="V10" s="10">
+        <v>18437024.999999989</v>
+      </c>
+      <c r="W10" s="3">
+        <v>760.99997023889375</v>
+      </c>
+      <c r="X10" s="11">
+        <v>14030575476.293732</v>
+      </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -1655,8 +1786,17 @@
       <c r="U11" s="3">
         <v>150</v>
       </c>
+      <c r="V11" s="10">
+        <v>101115264.99999997</v>
+      </c>
+      <c r="W11" s="3">
+        <v>638.26884422319938</v>
+      </c>
+      <c r="X11" s="11">
+        <v>64538723324.872505</v>
+      </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -1720,8 +1860,17 @@
       <c r="U12" s="3">
         <v>150</v>
       </c>
+      <c r="V12" s="10">
+        <v>6086280.0000000009</v>
+      </c>
+      <c r="W12" s="3">
+        <v>2419.1673936541579</v>
+      </c>
+      <c r="X12" s="11">
+        <v>14723730124.649429</v>
+      </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>34</v>
       </c>
@@ -1785,8 +1934,17 @@
       <c r="U13" s="3">
         <v>150</v>
       </c>
+      <c r="V13" s="10">
+        <v>29159502.999999996</v>
+      </c>
+      <c r="W13" s="3">
+        <v>2817.8811287763206</v>
+      </c>
+      <c r="X13" s="11">
+        <v>82168013228.196503</v>
+      </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>37</v>
       </c>
@@ -1850,8 +2008,17 @@
       <c r="U14" s="3">
         <v>150</v>
       </c>
+      <c r="V14" s="10">
+        <v>1043016.0000000001</v>
+      </c>
+      <c r="W14" s="3">
+        <v>3675.6189752318733</v>
+      </c>
+      <c r="X14" s="11">
+        <v>3833729401.0704479</v>
+      </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -1915,8 +2082,17 @@
       <c r="U15" s="3">
         <v>150</v>
       </c>
+      <c r="V15" s="10">
+        <v>109887164</v>
+      </c>
+      <c r="W15" s="3">
+        <v>4235.802789781611</v>
+      </c>
+      <c r="X15" s="11">
+        <v>465460355832.3894</v>
+      </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
@@ -1980,8 +2156,17 @@
       <c r="U16" s="3">
         <v>150</v>
       </c>
+      <c r="V16" s="10">
+        <v>1590203.9999999995</v>
+      </c>
+      <c r="W16" s="3">
+        <v>9246.96875410752</v>
+      </c>
+      <c r="X16" s="11">
+        <v>14704566700.65679</v>
+      </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>46</v>
       </c>
@@ -2045,8 +2230,17 @@
       <c r="U17" s="3">
         <v>150</v>
       </c>
+      <c r="V17" s="10">
+        <v>3795984.0000000009</v>
+      </c>
+      <c r="W17" s="3">
+        <v>689.04304984399994</v>
+      </c>
+      <c r="X17" s="11">
+        <v>2615596392.5190268</v>
+      </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>49</v>
       </c>
@@ -2110,8 +2304,17 @@
       <c r="U18" s="3">
         <v>150</v>
       </c>
+      <c r="V18" s="10">
+        <v>1210452.0000000002</v>
+      </c>
+      <c r="W18" s="3">
+        <v>4605.6931675416017</v>
+      </c>
+      <c r="X18" s="11">
+        <v>5574970506.0370684</v>
+      </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>52</v>
       </c>
@@ -2175,8 +2378,17 @@
       <c r="U19" s="3">
         <v>150</v>
       </c>
+      <c r="V19" s="10">
+        <v>126750867.99999991</v>
+      </c>
+      <c r="W19" s="3">
+        <v>1031.4967902263556</v>
+      </c>
+      <c r="X19" s="11">
+        <v>130743113500.4044</v>
+      </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>55</v>
       </c>
@@ -2240,8 +2452,17 @@
       <c r="U20" s="3">
         <v>150</v>
       </c>
+      <c r="V20" s="10">
+        <v>2435945.0000000009</v>
+      </c>
+      <c r="W20" s="3">
+        <v>8760.3819731424155</v>
+      </c>
+      <c r="X20" s="11">
+        <v>21339808665.56641</v>
+      </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>58</v>
       </c>
@@ -2305,8 +2526,17 @@
       <c r="U21" s="3">
         <v>150</v>
       </c>
+      <c r="V21" s="10">
+        <v>2705194.0000000005</v>
+      </c>
+      <c r="W21" s="3">
+        <v>913.07658530156198</v>
+      </c>
+      <c r="X21" s="11">
+        <v>2470049300.0982742</v>
+      </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>61</v>
       </c>
@@ -2370,8 +2600,17 @@
       <c r="U22" s="3">
         <v>150</v>
       </c>
+      <c r="V22" s="10">
+        <v>33733902.000000007</v>
+      </c>
+      <c r="W22" s="3">
+        <v>2672.0352246405087</v>
+      </c>
+      <c r="X22" s="11">
+        <v>90138174408.570923</v>
+      </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>64</v>
       </c>
@@ -2435,8 +2674,17 @@
       <c r="U23" s="3">
         <v>150</v>
       </c>
+      <c r="V23" s="10">
+        <v>14617783.999999994</v>
+      </c>
+      <c r="W23" s="3">
+        <v>1283.2471999743909</v>
+      </c>
+      <c r="X23" s="11">
+        <v>18758230387.830444</v>
+      </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>67</v>
       </c>
@@ -2500,8 +2748,17 @@
       <c r="U24" s="3">
         <v>150</v>
       </c>
+      <c r="V24" s="10">
+        <v>2160279.9999999991</v>
+      </c>
+      <c r="W24" s="3">
+        <v>888.34593496511081</v>
+      </c>
+      <c r="X24" s="11">
+        <v>1919075956.3864288</v>
+      </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>70</v>
       </c>
@@ -2565,8 +2822,17 @@
       <c r="U25" s="3">
         <v>150</v>
       </c>
+      <c r="V25" s="10">
+        <v>58714808.999999978</v>
+      </c>
+      <c r="W25" s="3">
+        <v>2192.9197732123466</v>
+      </c>
+      <c r="X25" s="11">
+        <v>128756865636.48621</v>
+      </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>73</v>
       </c>
@@ -2630,8 +2896,17 @@
       <c r="U26" s="3">
         <v>150</v>
       </c>
+      <c r="V26" s="10">
+        <v>2209599.0000000023</v>
+      </c>
+      <c r="W26" s="3">
+        <v>1274.6241575173519</v>
+      </c>
+      <c r="X26" s="11">
+        <v>2816408263.8261862</v>
+      </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>76</v>
       </c>
@@ -2695,8 +2970,17 @@
       <c r="U27" s="3">
         <v>150</v>
       </c>
+      <c r="V27" s="10">
+        <v>5561376.9999999981</v>
+      </c>
+      <c r="W27" s="3">
+        <v>735.50259700305287</v>
+      </c>
+      <c r="X27" s="11">
+        <v>4090407226.4130459</v>
+      </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>79</v>
       </c>
@@ -2760,8 +3044,17 @@
       <c r="U28" s="3">
         <v>150</v>
       </c>
+      <c r="V28" s="10">
+        <v>7193917</v>
+      </c>
+      <c r="W28" s="3">
+        <v>6576.517576235141</v>
+      </c>
+      <c r="X28" s="11">
+        <v>47310921592.476776</v>
+      </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>82</v>
       </c>
@@ -2825,8 +3118,17 @@
       <c r="U29" s="3">
         <v>150</v>
       </c>
+      <c r="V29" s="10">
+        <v>21287587.999999996</v>
+      </c>
+      <c r="W29" s="3">
+        <v>702.24856361256707</v>
+      </c>
+      <c r="X29" s="11">
+        <v>14949178095.776117</v>
+      </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>85</v>
       </c>
@@ -2890,8 +3192,17 @@
       <c r="U30" s="3">
         <v>150</v>
       </c>
+      <c r="V30" s="10">
+        <v>22752839.999999996</v>
+      </c>
+      <c r="W30" s="3">
+        <v>1003.0283878665916</v>
+      </c>
+      <c r="X30" s="11">
+        <v>22821744424.586498</v>
+      </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>88</v>
       </c>
@@ -2955,8 +3266,17 @@
       <c r="U31" s="3">
         <v>150</v>
       </c>
+      <c r="V31" s="10">
+        <v>5159892.9999999953</v>
+      </c>
+      <c r="W31" s="3">
+        <v>1882.7837724833846</v>
+      </c>
+      <c r="X31" s="11">
+        <v>9714962808.1506004</v>
+      </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>91</v>
       </c>
@@ -3020,8 +3340,17 @@
       <c r="U32" s="3">
         <v>150</v>
       </c>
+      <c r="V32" s="10">
+        <v>38606160</v>
+      </c>
+      <c r="W32" s="3">
+        <v>3821.002207737793</v>
+      </c>
+      <c r="X32" s="11">
+        <v>147514222592.27847</v>
+      </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>94</v>
       </c>
@@ -3085,8 +3414,17 @@
       <c r="U33" s="3">
         <v>150</v>
       </c>
+      <c r="V33" s="10">
+        <v>34999755.999999978</v>
+      </c>
+      <c r="W33" s="3">
+        <v>546.84955428605815</v>
+      </c>
+      <c r="X33" s="11">
+        <v>19139600968.720776</v>
+      </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>97</v>
       </c>
@@ -3150,8 +3488,17 @@
       <c r="U34" s="3">
         <v>150</v>
       </c>
+      <c r="V34" s="10">
+        <v>2727257</v>
+      </c>
+      <c r="W34" s="3">
+        <v>5167.8020435604667</v>
+      </c>
+      <c r="X34" s="11">
+        <v>14093924297.914587</v>
+      </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>100</v>
       </c>
@@ -3215,8 +3562,17 @@
       <c r="U35" s="3">
         <v>150</v>
       </c>
+      <c r="V35" s="10">
+        <v>28079834.000000004</v>
+      </c>
+      <c r="W35" s="3">
+        <v>650.09072944156355</v>
+      </c>
+      <c r="X35" s="11">
+        <v>18254439767.65802</v>
+      </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>103</v>
       </c>
@@ -3280,8 +3636,17 @@
       <c r="U36" s="3">
         <v>150</v>
       </c>
+      <c r="V36" s="10">
+        <v>227713026.99999997</v>
+      </c>
+      <c r="W36" s="3">
+        <v>2278.3694125050547</v>
+      </c>
+      <c r="X36" s="11">
+        <v>518814395545.73761</v>
+      </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>106</v>
       </c>
@@ -3345,8 +3710,17 @@
       <c r="U37" s="3">
         <v>150</v>
       </c>
+      <c r="V37" s="10">
+        <v>14249748.000000006</v>
+      </c>
+      <c r="W37" s="3">
+        <v>911.1484185545238</v>
+      </c>
+      <c r="X37" s="11">
+        <v>12983635355.000494</v>
+      </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>109</v>
       </c>
@@ -3410,8 +3784,17 @@
       <c r="U38" s="3">
         <v>150</v>
       </c>
+      <c r="V38" s="10">
+        <v>18585815</v>
+      </c>
+      <c r="W38" s="3">
+        <v>1755.4353956616928</v>
+      </c>
+      <c r="X38" s="11">
+        <v>32626197508.220024</v>
+      </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>112</v>
       </c>
@@ -3475,8 +3858,17 @@
       <c r="U39" s="3">
         <v>150</v>
       </c>
+      <c r="V39" s="10">
+        <v>8638684.0000000019</v>
+      </c>
+      <c r="W39" s="3">
+        <v>563.77292691362845</v>
+      </c>
+      <c r="X39" s="11">
+        <v>4870256163.3619328</v>
+      </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>115</v>
       </c>
@@ -3540,8 +3932,17 @@
       <c r="U40" s="3">
         <v>150</v>
       </c>
+      <c r="V40" s="10">
+        <v>17851254.999999996</v>
+      </c>
+      <c r="W40" s="3">
+        <v>487.1147673341577</v>
+      </c>
+      <c r="X40" s="11">
+        <v>8695609925.9477177</v>
+      </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>118</v>
       </c>
@@ -3605,8 +4006,17 @@
       <c r="U41" s="3">
         <v>150</v>
       </c>
+      <c r="V41" s="10">
+        <v>62134218.000000037</v>
+      </c>
+      <c r="W41" s="3">
+        <v>7642.7639175561035</v>
+      </c>
+      <c r="X41" s="11">
+        <v>474877159375.96527</v>
+      </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>121</v>
       </c>
@@ -3670,8 +4080,17 @@
       <c r="U42" s="3">
         <v>150</v>
       </c>
+      <c r="V42" s="10">
+        <v>12176470.999999998</v>
+      </c>
+      <c r="W42" s="3">
+        <v>398.17879153000007</v>
+      </c>
+      <c r="X42" s="11">
+        <v>4848412507.8800907</v>
+      </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>124</v>
       </c>
@@ -3735,8 +4154,17 @@
       <c r="U43" s="3">
         <v>150</v>
       </c>
+      <c r="V43" s="10">
+        <v>48216428.999999978</v>
+      </c>
+      <c r="W43" s="3">
+        <v>835.21605164190703</v>
+      </c>
+      <c r="X43" s="11">
+        <v>40271135453.652328</v>
+      </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>127</v>
       </c>
@@ -3800,8 +4228,17 @@
       <c r="U44" s="3">
         <v>150</v>
       </c>
+      <c r="V44" s="10">
+        <v>67014130.000000045</v>
+      </c>
+      <c r="W44" s="3">
+        <v>1240.8348600960667</v>
+      </c>
+      <c r="X44" s="11">
+        <v>83153468623.009674</v>
+      </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>130</v>
       </c>
@@ -3865,8 +4302,17 @@
       <c r="U45" s="3">
         <v>150</v>
       </c>
+      <c r="V45" s="10">
+        <v>9095785.0000000075</v>
+      </c>
+      <c r="W45" s="3">
+        <v>1084.3440676319865</v>
+      </c>
+      <c r="X45" s="11">
+        <v>9862960505.2060165</v>
+      </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>133</v>
       </c>
@@ -3930,8 +4376,17 @@
       <c r="U46" s="3">
         <v>150</v>
       </c>
+      <c r="V46" s="10">
+        <v>12251377.999999994</v>
+      </c>
+      <c r="W46" s="3">
+        <v>4288.2365639374202</v>
+      </c>
+      <c r="X46" s="11">
+        <v>52536807098.218483</v>
+      </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>136</v>
       </c>
@@ -3995,8 +4450,17 @@
       <c r="U47" s="3">
         <v>150</v>
       </c>
+      <c r="V47" s="10">
+        <v>50976034.000000015</v>
+      </c>
+      <c r="W47" s="3">
+        <v>937.62261171112254</v>
+      </c>
+      <c r="X47" s="11">
+        <v>47796282133.754997</v>
+      </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>139</v>
       </c>
@@ -4060,8 +4524,17 @@
       <c r="U48" s="3">
         <v>150</v>
       </c>
+      <c r="V48" s="10">
+        <v>20608355.999999996</v>
+      </c>
+      <c r="W48" s="3">
+        <v>1224.54284434702</v>
+      </c>
+      <c r="X48" s="11">
+        <v>25235814873.555973</v>
+      </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>142</v>
       </c>
@@ -4124,6 +4597,15 @@
       </c>
       <c r="U49" s="3">
         <v>150</v>
+      </c>
+      <c r="V49" s="10">
+        <v>15840801.999999994</v>
+      </c>
+      <c r="W49" s="3">
+        <v>1898.2569083438891</v>
+      </c>
+      <c r="X49" s="11">
+        <v>30069911830.207684</v>
       </c>
     </row>
   </sheetData>
@@ -4132,14 +4614,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView topLeftCell="R1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AO36" sqref="AO36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:49" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>